<commit_message>
update the tm tracker w/ more options
</commit_message>
<xml_diff>
--- a/trackers/-10 TM Tracker.xlsx
+++ b/trackers/-10 TM Tracker.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicho\OneDrive\Desktop\Dev Projects\TM-Generator\trackers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83CDDD32-23D7-4930-A3E1-DE036D0E9F82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1699B72-B68D-4426-9067-D24A30438C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2660" yWindow="2660" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="-10" sheetId="1" r:id="rId1"/>
+    <sheet name="Chapters" sheetId="2" r:id="rId2"/>
+    <sheet name="Procedures" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="140">
   <si>
     <t>WP NO:</t>
   </si>
@@ -61,9 +63,6 @@
     <t>Theory of Operation</t>
   </si>
   <si>
-    <t>Chapter 2 - Operator Procedures</t>
-  </si>
-  <si>
     <t>O00001</t>
   </si>
   <si>
@@ -94,18 +93,12 @@
     <t>Operation Under Unusual Conditions</t>
   </si>
   <si>
-    <t>Chapter 3 - Troubleshooting Master Index</t>
-  </si>
-  <si>
     <t>T00000</t>
   </si>
   <si>
     <t>Troubleshooting Index</t>
   </si>
   <si>
-    <t>Chapter 4 - Operator Troubleshooting</t>
-  </si>
-  <si>
     <t>T00001</t>
   </si>
   <si>
@@ -136,9 +129,6 @@
     <t>Water Faults</t>
   </si>
   <si>
-    <t>Chapter 5 - Operator PMCS</t>
-  </si>
-  <si>
     <t>M00001</t>
   </si>
   <si>
@@ -169,69 +159,42 @@
     <t>PMCS Annually</t>
   </si>
   <si>
-    <t>Chapter 6 - Operator Maintenance</t>
-  </si>
-  <si>
     <t>M00006</t>
   </si>
   <si>
     <t>Emergency Stop</t>
   </si>
   <si>
-    <t>Remove</t>
-  </si>
-  <si>
     <t>M00007</t>
   </si>
   <si>
     <t>Assembly</t>
   </si>
   <si>
-    <t>Service</t>
-  </si>
-  <si>
     <t>M00008</t>
   </si>
   <si>
-    <t>Install</t>
-  </si>
-  <si>
     <t>M00009</t>
   </si>
   <si>
     <t>Cargo Door</t>
   </si>
   <si>
-    <t>Repair</t>
-  </si>
-  <si>
     <t>M00010</t>
   </si>
   <si>
     <t>Shelter</t>
   </si>
   <si>
-    <t>Prepforuse</t>
-  </si>
-  <si>
     <t>M00011</t>
   </si>
   <si>
-    <t>Transport</t>
-  </si>
-  <si>
     <t>M00012</t>
   </si>
   <si>
     <t>Braising Pans</t>
   </si>
   <si>
-    <t>Clean</t>
-  </si>
-  <si>
-    <t>Chapter 7 - Destruction of Equipment to Prevent Enemy Use</t>
-  </si>
-  <si>
     <t>D00001</t>
   </si>
   <si>
@@ -250,9 +213,6 @@
     <t>Destruction of Equipment to Prevent Enemy Use Procedure 2</t>
   </si>
   <si>
-    <t>Chapter 8 - Supporting Information</t>
-  </si>
-  <si>
     <t>S00001</t>
   </si>
   <si>
@@ -320,6 +280,168 @@
   </si>
   <si>
     <t>How to use this Manual</t>
+  </si>
+  <si>
+    <t>Operator Procedures</t>
+  </si>
+  <si>
+    <t>Troubleshooting Master Index</t>
+  </si>
+  <si>
+    <t>Operator Troubleshooting</t>
+  </si>
+  <si>
+    <t>Operator PMCS</t>
+  </si>
+  <si>
+    <t>Operator Maintenance</t>
+  </si>
+  <si>
+    <t>Destruction of Equipment to Prevent Enemy Use</t>
+  </si>
+  <si>
+    <t>Supporting Information</t>
+  </si>
+  <si>
+    <t>Chapter</t>
+  </si>
+  <si>
+    <t>inspect</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>service</t>
+  </si>
+  <si>
+    <t>adjust</t>
+  </si>
+  <si>
+    <t>align</t>
+  </si>
+  <si>
+    <t>remove</t>
+  </si>
+  <si>
+    <t>install</t>
+  </si>
+  <si>
+    <t>replace</t>
+  </si>
+  <si>
+    <t>repair</t>
+  </si>
+  <si>
+    <t>paint</t>
+  </si>
+  <si>
+    <t>overhaul</t>
+  </si>
+  <si>
+    <t>rebuild</t>
+  </si>
+  <si>
+    <t>mark</t>
+  </si>
+  <si>
+    <t>pack</t>
+  </si>
+  <si>
+    <t>unpack</t>
+  </si>
+  <si>
+    <t>prepforuse</t>
+  </si>
+  <si>
+    <t>clean</t>
+  </si>
+  <si>
+    <t>assem</t>
+  </si>
+  <si>
+    <t>disassem</t>
+  </si>
+  <si>
+    <t>ndi</t>
+  </si>
+  <si>
+    <t>ris</t>
+  </si>
+  <si>
+    <t>pis</t>
+  </si>
+  <si>
+    <t>tow</t>
+  </si>
+  <si>
+    <t>jack</t>
+  </si>
+  <si>
+    <t>park</t>
+  </si>
+  <si>
+    <t>moor</t>
+  </si>
+  <si>
+    <t>cover</t>
+  </si>
+  <si>
+    <t>hoist</t>
+  </si>
+  <si>
+    <t>sling</t>
+  </si>
+  <si>
+    <t>extpwr</t>
+  </si>
+  <si>
+    <t>prepstore</t>
+  </si>
+  <si>
+    <t>prepship</t>
+  </si>
+  <si>
+    <t>transport</t>
+  </si>
+  <si>
+    <t>arm</t>
+  </si>
+  <si>
+    <t>load</t>
+  </si>
+  <si>
+    <t>calibration</t>
+  </si>
+  <si>
+    <t>lube</t>
+  </si>
+  <si>
+    <t>preservation</t>
+  </si>
+  <si>
+    <t>unload</t>
+  </si>
+  <si>
+    <t>installperdev</t>
+  </si>
+  <si>
+    <t>uninstallperdev</t>
+  </si>
+  <si>
+    <t>upgrade</t>
+  </si>
+  <si>
+    <t>configure</t>
+  </si>
+  <si>
+    <t>debug</t>
+  </si>
+  <si>
+    <t>Procedures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                                                                 </t>
   </si>
 </sst>
 </file>
@@ -348,7 +470,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -360,13 +482,8 @@
         <fgColor rgb="FFED7D31"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7F7F7F"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -396,11 +513,65 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -417,15 +588,21 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -443,6 +620,26 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{77DC6E53-A4E2-47FB-94F7-F26611073301}" name="Table4" displayName="Table4" ref="A1:A10" totalsRowShown="0">
+  <autoFilter ref="A1:A10" xr:uid="{77DC6E53-A4E2-47FB-94F7-F26611073301}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{F06D3B53-80FA-4A02-8757-A0309BE54380}" name="Chapter"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{35B06D75-B185-4D44-9F87-E9B47BFEB93B}" name="Table5" displayName="Table5" ref="A1:A45" totalsRowShown="0">
+  <autoFilter ref="A1:A45" xr:uid="{35B06D75-B185-4D44-9F87-E9B47BFEB93B}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{116829D8-8C19-4C56-A598-BEAC07DC2D35}" name="Procedures"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -736,20 +933,20 @@
   <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.453125" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="57.453125" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="57.453125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -789,7 +986,7 @@
       <c r="A5" s="1"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="D5" s="3"/>
     </row>
@@ -797,7 +994,7 @@
       <c r="A6" s="1"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="D6" s="3"/>
     </row>
@@ -805,7 +1002,7 @@
       <c r="A7" s="1"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="D7" s="3"/>
     </row>
@@ -851,57 +1048,57 @@
       <c r="A12" s="1"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="D17" s="3"/>
     </row>
@@ -909,17 +1106,17 @@
       <c r="A18" s="1"/>
       <c r="B18" s="4"/>
       <c r="C18" s="5" t="s">
-        <v>24</v>
+        <v>87</v>
       </c>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D19" s="3"/>
     </row>
@@ -927,57 +1124,57 @@
       <c r="A20" s="1"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
       <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D25" s="3"/>
     </row>
@@ -985,57 +1182,57 @@
       <c r="A26" s="1"/>
       <c r="B26" s="4"/>
       <c r="C26" s="5" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="3" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="B30" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D31" s="3"/>
     </row>
@@ -1043,239 +1240,578 @@
       <c r="A32" s="1"/>
       <c r="B32" s="4"/>
       <c r="C32" s="5" t="s">
-        <v>49</v>
+        <v>90</v>
       </c>
       <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="B34" s="3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
       <c r="B36" s="3" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>60</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
-      <c r="B37" s="3" t="s">
-        <v>61</v>
+      <c r="B37" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
-      <c r="B38" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>65</v>
+      <c r="B38" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
-      <c r="B39" s="1" t="s">
-        <v>66</v>
+      <c r="B39" s="11" t="s">
+        <v>55</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>68</v>
+        <v>56</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D40" s="6"/>
+      <c r="B40" s="10"/>
+      <c r="C40" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="10"/>
     </row>
     <row r="41" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="8"/>
+      <c r="A41" s="6"/>
       <c r="B41" s="3" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="8"/>
+      <c r="A42" s="6"/>
       <c r="B42" s="3" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="D42" s="3"/>
     </row>
     <row r="43" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="8"/>
+      <c r="A43" s="6"/>
       <c r="B43" s="3" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="8"/>
+      <c r="A44" s="6"/>
       <c r="B44" s="4"/>
       <c r="C44" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" s="4"/>
+    </row>
+    <row r="45" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="6"/>
+      <c r="B45" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="6"/>
+      <c r="B46" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="6"/>
+      <c r="B47" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47" s="3"/>
+    </row>
+    <row r="48" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="6"/>
+      <c r="B48" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="6"/>
+      <c r="B49" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="6"/>
+      <c r="B50" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D50" s="3"/>
+    </row>
+    <row r="51" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="6"/>
+      <c r="B51" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D44" s="4"/>
-    </row>
-    <row r="45" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="8"/>
-      <c r="B45" s="3" t="s">
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="6"/>
+      <c r="B52" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C52" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D45" s="3"/>
-    </row>
-    <row r="46" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="8"/>
-      <c r="B46" s="3" t="s">
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="6"/>
+      <c r="B53" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C53" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D46" s="3"/>
-    </row>
-    <row r="47" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="8"/>
-      <c r="B47" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D47" s="3"/>
-    </row>
-    <row r="48" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="8"/>
-      <c r="B48" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D48" s="3"/>
-    </row>
-    <row r="49" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="8"/>
-      <c r="B49" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D49" s="3"/>
-    </row>
-    <row r="50" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="8"/>
-      <c r="B50" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D50" s="3"/>
-    </row>
-    <row r="51" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="8"/>
-      <c r="B51" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D51" s="3"/>
-    </row>
-    <row r="52" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="8"/>
-      <c r="B52" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D52" s="3"/>
-    </row>
-    <row r="53" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="8"/>
-      <c r="B53" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="D53" s="3"/>
     </row>
     <row r="54" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="8"/>
+      <c r="A54" s="6"/>
       <c r="B54" s="4"/>
       <c r="C54" s="5" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="D54" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CEEF674F-9E1D-4069-8466-3956D4458B73}">
+          <x14:formula1>
+            <xm:f>Chapters!$A$2:$A$10</xm:f>
+          </x14:formula1>
+          <xm:sqref>C8 C12 C18 C20 C26 C32 C40 C44 C54</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{94A18E32-43BC-49F4-935D-194821316D28}">
+          <x14:formula1>
+            <xm:f>Procedures!$A$2:$A$45</xm:f>
+          </x14:formula1>
+          <xm:sqref>D33:D39</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C671AC-1638-4DF9-BBA7-DF57973D3C8B}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="43.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76C1A9BE-B36C-4637-A38E-7392AD4D6B59}">
+  <dimension ref="A1:D45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>